<commit_message>
fix: fix utf-8 bug in choose.py; update res.xlsx
</commit_message>
<xml_diff>
--- a/res-example/lab-result-empty.xlsx
+++ b/res-example/lab-result-empty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\上海交通大学\SJTU\助教\2025 春 Python\HomeworkMarking\res-example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C881154-0867-4CBD-90AF-234293B0DDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8F9863-9337-4007-AD06-96FC90E0C923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1416" yWindow="900" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -730,7 +730,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>